<commit_message>
add analyse for 200 dim
</commit_message>
<xml_diff>
--- a/snml/models/results.xlsx
+++ b/snml/models/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungp\Projects\word2vec\skip-gram\snml\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600AFAE1-4410-4C2B-AC95-AC25754050C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A14BCF7-26F9-4C4B-B3A6-9AB3170F8A46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,6 +418,9 @@
       <c r="D2">
         <v>7.97056833699029</v>
       </c>
+      <c r="E2">
+        <v>7.7457426577087602</v>
+      </c>
       <c r="I2">
         <v>50</v>
       </c>
@@ -439,6 +442,9 @@
       <c r="D3">
         <v>8.2471089866662801</v>
       </c>
+      <c r="E3">
+        <v>8.1820466466462101</v>
+      </c>
       <c r="I3">
         <v>100</v>
       </c>
@@ -460,6 +466,9 @@
       <c r="D4">
         <v>10.682056251980899</v>
       </c>
+      <c r="E4">
+        <v>10.811187772290999</v>
+      </c>
       <c r="I4">
         <v>150</v>
       </c>
@@ -481,8 +490,15 @@
       <c r="D5">
         <v>5.7844383738410503</v>
       </c>
+      <c r="E5">
+        <v>6.1052198352048697</v>
+      </c>
       <c r="I5">
         <v>200</v>
+      </c>
+      <c r="J5">
+        <f>SUM(E2:E101)</f>
+        <v>806.01100674742361</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -498,6 +514,9 @@
       <c r="D6">
         <v>8.3748167453195297</v>
       </c>
+      <c r="E6">
+        <v>8.2047055236769104</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -512,6 +531,9 @@
       <c r="D7">
         <v>8.6044969597479994</v>
       </c>
+      <c r="E7">
+        <v>8.5733498451961498</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -526,6 +548,9 @@
       <c r="D8">
         <v>9.3782901406499004</v>
       </c>
+      <c r="E8">
+        <v>9.0887143001191504</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -540,6 +565,9 @@
       <c r="D9">
         <v>6.4236320626197303</v>
       </c>
+      <c r="E9">
+        <v>6.0708631950241303</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -554,6 +582,9 @@
       <c r="D10">
         <v>10.6452283075406</v>
       </c>
+      <c r="E10">
+        <v>9.0858938706071992</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -568,6 +599,9 @@
       <c r="D11">
         <v>6.8167447878548497</v>
       </c>
+      <c r="E11">
+        <v>7.3296333595209298</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -582,6 +616,9 @@
       <c r="D12">
         <v>9.0397890518840196</v>
       </c>
+      <c r="E12">
+        <v>8.81801106108081</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -596,6 +633,9 @@
       <c r="D13">
         <v>7.7168987624060801</v>
       </c>
+      <c r="E13">
+        <v>7.8025429391290198</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -610,6 +650,9 @@
       <c r="D14">
         <v>9.6930803896419899</v>
       </c>
+      <c r="E14">
+        <v>9.6149293319806404</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -624,6 +667,9 @@
       <c r="D15">
         <v>11.8707453130248</v>
       </c>
+      <c r="E15">
+        <v>11.775094652976801</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -638,8 +684,11 @@
       <c r="D16">
         <v>9.7611443446701092</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>9.7855108843269303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -652,8 +701,11 @@
       <c r="D17">
         <v>8.0174484280899403</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>8.5274882585512994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -666,8 +718,11 @@
       <c r="D18">
         <v>8.7567339253731298</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>8.56497860968196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -680,8 +735,11 @@
       <c r="D19">
         <v>6.0108307650813897</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>5.90623373574683</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -694,8 +752,11 @@
       <c r="D20">
         <v>8.9508973339421498</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>9.0935389698429301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -708,8 +769,11 @@
       <c r="D21">
         <v>10.770779755594299</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>10.2739287882243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -722,8 +786,11 @@
       <c r="D22">
         <v>9.2759796626046604</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>8.9997149517471993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -736,8 +803,11 @@
       <c r="D23">
         <v>6.2381429001677997</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>6.1402302133352604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -750,8 +820,11 @@
       <c r="D24">
         <v>9.5108023018830696</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>9.3191864874357808</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -764,8 +837,11 @@
       <c r="D25">
         <v>5.7062249265419602</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>6.0687854439420397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -778,8 +854,11 @@
       <c r="D26">
         <v>9.5684567317462808</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>9.9976479762126491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -792,8 +871,11 @@
       <c r="D27">
         <v>7.5411841295155098</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>7.9419353418932603</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -806,8 +888,11 @@
       <c r="D28">
         <v>7.5758866258170103</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>7.31524257084049</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -820,8 +905,11 @@
       <c r="D29">
         <v>7.9589295277729297</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>7.8506857705436799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -834,8 +922,11 @@
       <c r="D30">
         <v>10.8423423131226</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>11.292999483616899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -848,8 +939,11 @@
       <c r="D31">
         <v>8.2213242599307303</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>9.8276519524951507</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -862,8 +956,11 @@
       <c r="D32">
         <v>6.5109595316711397</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>6.5367018784041298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -876,8 +973,11 @@
       <c r="D33">
         <v>6.1700525549036298</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>6.3416432398727904</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -890,8 +990,11 @@
       <c r="D34">
         <v>8.3236514036160898</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>8.1988823037354805</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -904,8 +1007,11 @@
       <c r="D35">
         <v>6.1491718445915096</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>6.0429664377289303</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -918,8 +1024,11 @@
       <c r="D36">
         <v>6.2189681337998</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>6.4193813025542301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -932,8 +1041,11 @@
       <c r="D37">
         <v>7.8794852306656997</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>8.1543849134463304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -946,8 +1058,11 @@
       <c r="D38">
         <v>10.8810905048196</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>10.703220971709399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -960,8 +1075,11 @@
       <c r="D39">
         <v>10.407464685929201</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>10.176015706808901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -974,8 +1092,11 @@
       <c r="D40">
         <v>7.3220643929209999</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>7.0373328733854201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -988,8 +1109,11 @@
       <c r="D41">
         <v>10.7713623456451</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>9.8341837482090604</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1002,8 +1126,11 @@
       <c r="D42">
         <v>7.2329516986699698</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>7.5532912599498401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1016,8 +1143,11 @@
       <c r="D43">
         <v>8.2618008991420293</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>8.4571832473338606</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1030,8 +1160,11 @@
       <c r="D44">
         <v>8.4998264119286109</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>8.2881944474525593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1044,8 +1177,11 @@
       <c r="D45">
         <v>7.4892047737955902</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>7.4034018823657197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1058,8 +1194,11 @@
       <c r="D46">
         <v>6.5322583348803196</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>6.4453679248901103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1072,8 +1211,11 @@
       <c r="D47">
         <v>10.4222167264685</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>10.4554480687733</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1086,8 +1228,11 @@
       <c r="D48">
         <v>7.5363904979121896</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>7.7843531472216796</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1100,8 +1245,11 @@
       <c r="D49">
         <v>5.9044209369273801</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>5.9227044388410803</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1114,8 +1262,11 @@
       <c r="D50">
         <v>9.5293144243994394</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>9.3410469855445406</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1128,8 +1279,11 @@
       <c r="D51">
         <v>12.841001157253499</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51">
+        <v>12.6219178811295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1142,8 +1296,11 @@
       <c r="D52">
         <v>8.1922126497280292</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52">
+        <v>8.0646015532704407</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1156,8 +1313,11 @@
       <c r="D53">
         <v>5.7147698963254197</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53">
+        <v>5.7105873714267501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1170,8 +1330,11 @@
       <c r="D54">
         <v>6.0321746967378704</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54">
+        <v>6.1879296999164097</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1184,8 +1347,11 @@
       <c r="D55">
         <v>8.3992795418269299</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55">
+        <v>8.3134088008801506</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1198,8 +1364,11 @@
       <c r="D56">
         <v>5.71154856349012</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>5.5966469831860399</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1212,8 +1381,11 @@
       <c r="D57">
         <v>6.1254230665451397</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>6.6018126848826997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1226,8 +1398,11 @@
       <c r="D58">
         <v>8.3516495604971102</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>8.3064568917505497</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1240,8 +1415,11 @@
       <c r="D59">
         <v>10.9460995375493</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59">
+        <v>10.572120618299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1254,8 +1432,11 @@
       <c r="D60">
         <v>8.9613656866480795</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>8.5592281578326403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1268,8 +1449,11 @@
       <c r="D61">
         <v>8.3939503284303107</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>8.3574681860665301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1282,8 +1466,11 @@
       <c r="D62">
         <v>8.1829830559315706</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>8.3254602330427492</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1296,8 +1483,11 @@
       <c r="D63">
         <v>6.2055993154873903</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>6.3334929301802401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1310,8 +1500,11 @@
       <c r="D64">
         <v>11.976778253214</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64">
+        <v>11.673032078716799</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1324,8 +1517,11 @@
       <c r="D65">
         <v>9.8406166457282698</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>9.5216885802995197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1338,8 +1534,11 @@
       <c r="D66">
         <v>7.87852215175523</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66">
+        <v>7.6019952781847504</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1352,8 +1551,11 @@
       <c r="D67">
         <v>7.4337134726986402</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67">
+        <v>6.8211616531356603</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1366,8 +1568,11 @@
       <c r="D68">
         <v>10.159693714328901</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>9.7289000413689699</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1380,8 +1585,11 @@
       <c r="D69">
         <v>6.8088485620632797</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>6.3487825077506397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1394,8 +1602,11 @@
       <c r="D70">
         <v>8.4979707284019295</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>8.8039621188160897</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1408,8 +1619,11 @@
       <c r="D71">
         <v>10.002933259778199</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>10.0715930135442</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1422,8 +1636,11 @@
       <c r="D72">
         <v>5.5998053929350302</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>5.5548422756593796</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1436,8 +1653,11 @@
       <c r="D73">
         <v>6.7606949434011803</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>7.2148341461403804</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1450,8 +1670,11 @@
       <c r="D74">
         <v>8.5116593911501397</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>8.3913704158131601</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1464,8 +1687,11 @@
       <c r="D75">
         <v>7.1903551420220904</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>7.0432336727387899</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1478,8 +1704,11 @@
       <c r="D76">
         <v>5.5691746873162096</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E76">
+        <v>5.8304396598621704</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1492,8 +1721,11 @@
       <c r="D77">
         <v>6.1054735990321296</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>6.01909317416579</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1506,8 +1738,11 @@
       <c r="D78">
         <v>5.1936093790181204</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>5.1434050455112397</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1520,8 +1755,11 @@
       <c r="D79">
         <v>7.4093539962195196</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>7.3854603203904201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1534,8 +1772,11 @@
       <c r="D80">
         <v>8.9890095503333107</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E80">
+        <v>9.12206404135555</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1548,8 +1789,11 @@
       <c r="D81">
         <v>6.6233993320574402</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>6.7714409710330301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1562,8 +1806,11 @@
       <c r="D82">
         <v>9.0680466993140794</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>9.1640824865928199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1576,8 +1823,11 @@
       <c r="D83">
         <v>8.3660209000646102</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>8.1484429606630702</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1590,8 +1840,11 @@
       <c r="D84">
         <v>5.8574336260101401</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E84">
+        <v>6.0958563559075296</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1604,8 +1857,11 @@
       <c r="D85">
         <v>7.6110359476045497</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E85">
+        <v>7.9907401244064404</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1618,8 +1874,11 @@
       <c r="D86">
         <v>7.35466312324243</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E86">
+        <v>7.3869622606978496</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1632,8 +1891,11 @@
       <c r="D87">
         <v>7.1360712328317701</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E87">
+        <v>7.4827916873056104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1646,8 +1908,11 @@
       <c r="D88">
         <v>6.7353427452692802</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E88">
+        <v>6.71050811463763</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1660,8 +1925,11 @@
       <c r="D89">
         <v>11.9998790193648</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E89">
+        <v>12.3594170126203</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1674,8 +1942,11 @@
       <c r="D90">
         <v>4.3547290852238598</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E90">
+        <v>3.6822386377104999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1688,8 +1959,11 @@
       <c r="D91">
         <v>8.3445165553476492</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E91">
+        <v>8.6333916978682197</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1702,8 +1976,11 @@
       <c r="D92">
         <v>9.9391748030366198</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E92">
+        <v>9.7771992139937591</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1716,8 +1993,11 @@
       <c r="D93">
         <v>6.4850593933951002</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E93">
+        <v>6.3303983607575196</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1730,8 +2010,11 @@
       <c r="D94">
         <v>6.5912140211356203</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <v>6.8707368264093898</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1744,8 +2027,11 @@
       <c r="D95">
         <v>9.5466518976747494</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E95">
+        <v>9.2863833544322105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1758,8 +2044,11 @@
       <c r="D96">
         <v>8.0510748065870992</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E96">
+        <v>8.5346606335119297</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1772,8 +2061,11 @@
       <c r="D97">
         <v>8.6826853817854399</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97">
+        <v>8.5030060151334705</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1786,8 +2078,11 @@
       <c r="D98">
         <v>7.1027690135351804</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E98">
+        <v>7.1304089752655804</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1800,8 +2095,11 @@
       <c r="D99">
         <v>7.7955049469541198</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E99">
+        <v>7.5698404086488296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1814,8 +2112,11 @@
       <c r="D100">
         <v>8.0701023772931908</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E100">
+        <v>8.2172030702016503</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -1827,6 +2128,9 @@
       </c>
       <c r="D101">
         <v>6.3791866738332699</v>
+      </c>
+      <c r="E101">
+        <v>6.3289083564824198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>